<commit_message>
added pathologicalstate reference list
</commit_message>
<xml_diff>
--- a/dist/rd3_novelomics.xlsx
+++ b/dist/rd3_novelomics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="252">
   <si>
     <t>rd3</t>
   </si>
@@ -204,7 +204,10 @@
     <t>sex2</t>
   </si>
   <si>
-    <t>tissueStatus</t>
+    <t>pathologicalState</t>
+  </si>
+  <si>
+    <t>percentageTumorCells</t>
   </si>
   <si>
     <t>tissueType</t>
@@ -363,9 +366,6 @@
     <t>Observed sex</t>
   </si>
   <si>
-    <t>Tissue Status</t>
-  </si>
-  <si>
     <t>Tissue Types</t>
   </si>
   <si>
@@ -483,10 +483,10 @@
     <t>if deceased, age of death (COMMON DATA ELEMENTS 3.2)</t>
   </si>
   <si>
-    <t>Age at onset (COMMON DATA ELEMENTS 5.1)</t>
-  </si>
-  <si>
-    <t>Age at diagnosis  (COMMON DATA ELEMENTS 5.2)</t>
+    <t>Age at onset (COMMON DATA ELEMENTS 5.1)</t>
+  </si>
+  <si>
+    <t>Age at diagnosis (COMMON DATA ELEMENTS 5.2)</t>
   </si>
   <si>
     <t>country of origin (for pedigree?)</t>
@@ -513,7 +513,10 @@
     <t>Computed sex (based on Y- chromosome)</t>
   </si>
   <si>
-    <t>An indication whether or not the tissue is affected</t>
+    <t>The pathological state of the tissue from which this material was derived. (GO:0001894)</t>
+  </si>
+  <si>
+    <t>The percentage of tumor cells compared to total cells present in this material. (NCIT:C127771)</t>
   </si>
   <si>
     <t>material type. E.g. DNA</t>
@@ -609,9 +612,6 @@
     <t>Patch to which the labinfo belongs</t>
   </si>
   <si>
-    <t>$('clinical_status').eq(true).value()</t>
-  </si>
-  <si>
     <t>token</t>
   </si>
   <si>
@@ -648,12 +648,12 @@
     <t>categorical</t>
   </si>
   <si>
+    <t>decimal</t>
+  </si>
+  <si>
     <t>datetime</t>
   </si>
   <si>
-    <t>decimal</t>
-  </si>
-  <si>
     <t>rd3_sex</t>
   </si>
   <si>
@@ -673,6 +673,9 @@
   </si>
   <si>
     <t>rd3_patch</t>
+  </si>
+  <si>
+    <t>rd3_pathologicalstate</t>
   </si>
   <si>
     <t>rd3_tissueType</t>
@@ -1123,16 +1126,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1175,16 +1178,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1278,7 +1281,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S87"/>
+  <dimension ref="A1:S88"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1286,61 +1289,61 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:19">
@@ -1392,7 +1395,7 @@
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
         <v>135</v>
@@ -1433,7 +1436,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
         <v>136</v>
@@ -1477,7 +1480,7 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
         <v>137</v>
@@ -1518,7 +1521,7 @@
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
         <v>138</v>
@@ -1562,7 +1565,7 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
         <v>139</v>
@@ -1606,7 +1609,7 @@
         <v>35</v>
       </c>
       <c r="C8" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
         <v>140</v>
@@ -1655,8 +1658,8 @@
       <c r="E9" t="b">
         <v>1</v>
       </c>
-      <c r="F9" t="s">
-        <v>197</v>
+      <c r="F9" t="b">
+        <v>1</v>
       </c>
       <c r="G9" t="b">
         <v>0</v>
@@ -1864,7 +1867,7 @@
         <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D14" t="s">
         <v>145</v>
@@ -1993,7 +1996,7 @@
         <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D17" t="s">
         <v>147</v>
@@ -2034,7 +2037,7 @@
         <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
         <v>148</v>
@@ -2075,7 +2078,7 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E19" t="b">
         <v>1</v>
@@ -2113,7 +2116,7 @@
         <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D20" t="s">
         <v>149</v>
@@ -2157,7 +2160,7 @@
         <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
         <v>150</v>
@@ -2201,7 +2204,7 @@
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
         <v>151</v>
@@ -2234,7 +2237,7 @@
         <v>0</v>
       </c>
       <c r="Q22" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -2245,7 +2248,7 @@
         <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
         <v>152</v>
@@ -2289,10 +2292,10 @@
         <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E24" t="b">
         <v>1</v>
@@ -2371,7 +2374,7 @@
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D26" t="s">
         <v>135</v>
@@ -2418,7 +2421,7 @@
         <v>52</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D27" t="s">
         <v>153</v>
@@ -2585,7 +2588,7 @@
         <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D31" t="s">
         <v>157</v>
@@ -2626,7 +2629,7 @@
         <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D32" t="s">
         <v>158</v>
@@ -2667,7 +2670,7 @@
         <v>50</v>
       </c>
       <c r="C33" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
         <v>152</v>
@@ -2711,10 +2714,10 @@
         <v>51</v>
       </c>
       <c r="C34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D34" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E34" t="b">
         <v>1</v>
@@ -2963,7 +2966,7 @@
         <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D40" t="s">
         <v>136</v>
@@ -3007,7 +3010,7 @@
         <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D41" t="s">
         <v>164</v>
@@ -3050,9 +3053,6 @@
       <c r="B42" t="s">
         <v>62</v>
       </c>
-      <c r="C42" t="s">
-        <v>115</v>
-      </c>
       <c r="D42" t="s">
         <v>165</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L42" t="b">
         <v>0</v>
@@ -3082,6 +3082,9 @@
       </c>
       <c r="N42" t="b">
         <v>0</v>
+      </c>
+      <c r="O42" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -3091,8 +3094,8 @@
       <c r="B43" t="s">
         <v>63</v>
       </c>
-      <c r="C43" t="s">
-        <v>116</v>
+      <c r="D43" t="s">
+        <v>166</v>
       </c>
       <c r="E43" t="b">
         <v>1</v>
@@ -3110,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="K43" t="s">
-        <v>200</v>
+        <v>210</v>
       </c>
       <c r="L43" t="b">
         <v>0</v>
@@ -3120,9 +3123,6 @@
       </c>
       <c r="N43" t="b">
         <v>0</v>
-      </c>
-      <c r="O43" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -3133,7 +3133,7 @@
         <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E44" t="b">
         <v>1</v>
@@ -3151,7 +3151,7 @@
         <v>0</v>
       </c>
       <c r="K44" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L44" t="b">
         <v>0</v>
@@ -3161,6 +3161,9 @@
       </c>
       <c r="N44" t="b">
         <v>0</v>
+      </c>
+      <c r="O44" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:18">
@@ -3171,10 +3174,7 @@
         <v>65</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
-      </c>
-      <c r="D45" t="s">
-        <v>166</v>
+        <v>117</v>
       </c>
       <c r="E45" t="b">
         <v>1</v>
@@ -3192,7 +3192,7 @@
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L45" t="b">
         <v>0</v>
@@ -3202,9 +3202,6 @@
       </c>
       <c r="N45" t="b">
         <v>0</v>
-      </c>
-      <c r="O45" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="46" spans="1:18">
@@ -3215,7 +3212,7 @@
         <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="D46" t="s">
         <v>167</v>
@@ -3236,7 +3233,7 @@
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="L46" t="b">
         <v>0</v>
@@ -3246,6 +3243,9 @@
       </c>
       <c r="N46" t="b">
         <v>0</v>
+      </c>
+      <c r="O46" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:18">
@@ -3253,10 +3253,10 @@
         <v>25</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="D47" t="s">
         <v>168</v>
@@ -3277,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="K47" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="L47" t="b">
         <v>0</v>
@@ -3287,9 +3287,6 @@
       </c>
       <c r="N47" t="b">
         <v>0</v>
-      </c>
-      <c r="O47" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -3297,13 +3294,13 @@
         <v>25</v>
       </c>
       <c r="B48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D48" t="s">
-        <v>42</v>
+        <v>169</v>
       </c>
       <c r="E48" t="b">
         <v>1</v>
@@ -3333,7 +3330,7 @@
         <v>0</v>
       </c>
       <c r="O48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="49" spans="1:19">
@@ -3341,10 +3338,13 @@
         <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C49" t="s">
-        <v>119</v>
+        <v>42</v>
+      </c>
+      <c r="D49" t="s">
+        <v>42</v>
       </c>
       <c r="E49" t="b">
         <v>1</v>
@@ -3362,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="K49" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="L49" t="b">
         <v>0</v>
@@ -3373,11 +3373,8 @@
       <c r="N49" t="b">
         <v>0</v>
       </c>
-      <c r="Q49" t="s">
-        <v>228</v>
-      </c>
-      <c r="S49" t="s">
-        <v>230</v>
+      <c r="O49" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="50" spans="1:19">
@@ -3385,13 +3382,10 @@
         <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>120</v>
-      </c>
-      <c r="D50" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="E50" t="b">
         <v>1</v>
@@ -3409,7 +3403,7 @@
         <v>0</v>
       </c>
       <c r="K50" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="L50" t="b">
         <v>0</v>
@@ -3419,6 +3413,12 @@
       </c>
       <c r="N50" t="b">
         <v>0</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>229</v>
+      </c>
+      <c r="S50" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:19">
@@ -3429,7 +3429,10 @@
         <v>68</v>
       </c>
       <c r="C51" t="s">
-        <v>68</v>
+        <v>120</v>
+      </c>
+      <c r="D51" t="s">
+        <v>170</v>
       </c>
       <c r="E51" t="b">
         <v>1</v>
@@ -3447,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="K51" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="L51" t="b">
         <v>0</v>
@@ -3457,9 +3460,6 @@
       </c>
       <c r="N51" t="b">
         <v>0</v>
-      </c>
-      <c r="O51" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="52" spans="1:19">
@@ -3470,10 +3470,7 @@
         <v>69</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
-      </c>
-      <c r="D52" t="s">
-        <v>170</v>
+        <v>69</v>
       </c>
       <c r="E52" t="b">
         <v>1</v>
@@ -3491,7 +3488,7 @@
         <v>0</v>
       </c>
       <c r="K52" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L52" t="b">
         <v>0</v>
@@ -3501,6 +3498,9 @@
       </c>
       <c r="N52" t="b">
         <v>0</v>
+      </c>
+      <c r="O52" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:19">
@@ -3508,10 +3508,10 @@
         <v>25</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="D53" t="s">
         <v>171</v>
@@ -3532,7 +3532,7 @@
         <v>0</v>
       </c>
       <c r="K53" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="L53" t="b">
         <v>0</v>
@@ -3542,9 +3542,6 @@
       </c>
       <c r="N53" t="b">
         <v>0</v>
-      </c>
-      <c r="O53" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:19">
@@ -3552,13 +3549,13 @@
         <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" t="s">
         <v>109</v>
       </c>
       <c r="D54" t="s">
-        <v>109</v>
+        <v>172</v>
       </c>
       <c r="E54" t="b">
         <v>1</v>
@@ -3576,7 +3573,7 @@
         <v>0</v>
       </c>
       <c r="K54" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="L54" t="b">
         <v>0</v>
@@ -3586,29 +3583,32 @@
       </c>
       <c r="N54" t="b">
         <v>0</v>
+      </c>
+      <c r="O54" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:19">
       <c r="A55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B55" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D55" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="E55" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
       </c>
       <c r="G55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" t="b">
         <v>0</v>
@@ -3620,13 +3620,13 @@
         <v>199</v>
       </c>
       <c r="L55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M55" t="b">
-        <v>1</v>
-      </c>
-      <c r="R55" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N55" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:19">
@@ -3637,10 +3637,10 @@
         <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D56" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E56" t="b">
         <v>0</v>
@@ -3649,7 +3649,7 @@
         <v>1</v>
       </c>
       <c r="G56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I56" t="b">
         <v>0</v>
@@ -3661,13 +3661,13 @@
         <v>199</v>
       </c>
       <c r="L56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M56" t="b">
         <v>1</v>
       </c>
-      <c r="N56" t="b">
-        <v>0</v>
+      <c r="R56" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:19">
@@ -3678,13 +3678,13 @@
         <v>72</v>
       </c>
       <c r="C57" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D57" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="E57" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
@@ -3705,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="M57" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N57" t="b">
         <v>0</v>
@@ -3719,13 +3719,13 @@
         <v>73</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>124</v>
       </c>
       <c r="D58" t="s">
         <v>173</v>
       </c>
       <c r="E58" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F58" t="b">
         <v>1</v>
@@ -3734,13 +3734,13 @@
         <v>0</v>
       </c>
       <c r="I58" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J58" t="b">
         <v>0</v>
       </c>
       <c r="K58" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="L58" t="b">
         <v>0</v>
@@ -3750,9 +3750,6 @@
       </c>
       <c r="N58" t="b">
         <v>0</v>
-      </c>
-      <c r="O58" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="59" spans="1:19">
@@ -3769,7 +3766,7 @@
         <v>174</v>
       </c>
       <c r="E59" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
@@ -3778,13 +3775,13 @@
         <v>0</v>
       </c>
       <c r="I59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J59" t="b">
         <v>0</v>
       </c>
       <c r="K59" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="L59" t="b">
         <v>0</v>
@@ -3796,7 +3793,7 @@
         <v>0</v>
       </c>
       <c r="O59" t="s">
-        <v>25</v>
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:19">
@@ -3804,10 +3801,10 @@
         <v>26</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="D60" t="s">
         <v>175</v>
@@ -3828,7 +3825,7 @@
         <v>0</v>
       </c>
       <c r="K60" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="L60" t="b">
         <v>0</v>
@@ -3840,7 +3837,7 @@
         <v>0</v>
       </c>
       <c r="O60" t="s">
-        <v>218</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:19">
@@ -3848,13 +3845,13 @@
         <v>26</v>
       </c>
       <c r="B61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C61" t="s">
         <v>109</v>
       </c>
       <c r="D61" t="s">
-        <v>109</v>
+        <v>176</v>
       </c>
       <c r="E61" t="b">
         <v>1</v>
@@ -3872,7 +3869,7 @@
         <v>0</v>
       </c>
       <c r="K61" t="s">
-        <v>199</v>
+        <v>207</v>
       </c>
       <c r="L61" t="b">
         <v>0</v>
@@ -3882,6 +3879,9 @@
       </c>
       <c r="N61" t="b">
         <v>0</v>
+      </c>
+      <c r="O61" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="62" spans="1:19">
@@ -3889,13 +3889,13 @@
         <v>26</v>
       </c>
       <c r="B62" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="C62" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D62" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="E62" t="b">
         <v>1</v>
@@ -3913,7 +3913,7 @@
         <v>0</v>
       </c>
       <c r="K62" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="L62" t="b">
         <v>0</v>
@@ -3933,7 +3933,10 @@
         <v>76</v>
       </c>
       <c r="C63" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="D63" t="s">
+        <v>177</v>
       </c>
       <c r="E63" t="b">
         <v>1</v>
@@ -3951,7 +3954,7 @@
         <v>0</v>
       </c>
       <c r="K63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="L63" t="b">
         <v>0</v>
@@ -3971,7 +3974,7 @@
         <v>77</v>
       </c>
       <c r="C64" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="E64" t="b">
         <v>1</v>
@@ -3989,7 +3992,7 @@
         <v>0</v>
       </c>
       <c r="K64" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="L64" t="b">
         <v>0</v>
@@ -4009,10 +4012,7 @@
         <v>78</v>
       </c>
       <c r="C65" t="s">
-        <v>127</v>
-      </c>
-      <c r="D65" t="s">
-        <v>127</v>
+        <v>78</v>
       </c>
       <c r="E65" t="b">
         <v>1</v>
@@ -4044,16 +4044,16 @@
     </row>
     <row r="66" spans="1:18">
       <c r="A66" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" t="s">
         <v>79</v>
       </c>
       <c r="C66" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="D66" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="E66" t="b">
         <v>1</v>
@@ -4071,7 +4071,7 @@
         <v>0</v>
       </c>
       <c r="K66" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="L66" t="b">
         <v>0</v>
@@ -4081,9 +4081,6 @@
       </c>
       <c r="N66" t="b">
         <v>0</v>
-      </c>
-      <c r="Q66" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="67" spans="1:18">
@@ -4100,13 +4097,13 @@
         <v>178</v>
       </c>
       <c r="E67" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
       </c>
       <c r="G67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" t="b">
         <v>0</v>
@@ -4115,16 +4112,19 @@
         <v>0</v>
       </c>
       <c r="K67" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="L67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M67" t="b">
-        <v>1</v>
-      </c>
-      <c r="R67" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N67" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="68" spans="1:18">
@@ -4147,7 +4147,7 @@
         <v>1</v>
       </c>
       <c r="G68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I68" t="b">
         <v>0</v>
@@ -4156,19 +4156,16 @@
         <v>0</v>
       </c>
       <c r="K68" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L68" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M68" t="b">
-        <v>0</v>
-      </c>
-      <c r="N68" t="b">
-        <v>0</v>
-      </c>
-      <c r="O68" t="s">
-        <v>223</v>
+        <v>1</v>
+      </c>
+      <c r="R68" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:18">
@@ -4185,7 +4182,7 @@
         <v>180</v>
       </c>
       <c r="E69" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F69" t="b">
         <v>1</v>
@@ -4200,7 +4197,7 @@
         <v>0</v>
       </c>
       <c r="K69" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="L69" t="b">
         <v>0</v>
@@ -4210,6 +4207,9 @@
       </c>
       <c r="N69" t="b">
         <v>0</v>
+      </c>
+      <c r="O69" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="70" spans="1:18">
@@ -4241,7 +4241,7 @@
         <v>0</v>
       </c>
       <c r="K70" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L70" t="b">
         <v>0</v>
@@ -4251,9 +4251,6 @@
       </c>
       <c r="N70" t="b">
         <v>0</v>
-      </c>
-      <c r="O70" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:18">
@@ -4329,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="K72" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="L72" t="b">
         <v>0</v>
@@ -4339,6 +4336,9 @@
       </c>
       <c r="N72" t="b">
         <v>0</v>
+      </c>
+      <c r="O72" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="73" spans="1:18">
@@ -4370,7 +4370,7 @@
         <v>0</v>
       </c>
       <c r="K73" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="L73" t="b">
         <v>0</v>
@@ -4384,25 +4384,25 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B74" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="C74" t="s">
-        <v>29</v>
+        <v>87</v>
       </c>
       <c r="D74" t="s">
         <v>185</v>
       </c>
       <c r="E74" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74" t="b">
         <v>1</v>
       </c>
       <c r="G74" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" t="b">
         <v>0</v>
@@ -4411,7 +4411,7 @@
         <v>0</v>
       </c>
       <c r="K74" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="L74" t="b">
         <v>0</v>
@@ -4419,8 +4419,8 @@
       <c r="M74" t="b">
         <v>0</v>
       </c>
-      <c r="R74" t="b">
-        <v>1</v>
+      <c r="N74" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:18">
@@ -4428,10 +4428,10 @@
         <v>28</v>
       </c>
       <c r="B75" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="C75" t="s">
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="D75" t="s">
         <v>186</v>
@@ -4443,7 +4443,7 @@
         <v>1</v>
       </c>
       <c r="G75" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I75" t="b">
         <v>0</v>
@@ -4455,13 +4455,13 @@
         <v>199</v>
       </c>
       <c r="L75" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M75" t="b">
-        <v>1</v>
-      </c>
-      <c r="N75" t="b">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="R75" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:18">
@@ -4469,16 +4469,16 @@
         <v>28</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="C76" t="s">
-        <v>7</v>
+        <v>78</v>
       </c>
       <c r="D76" t="s">
         <v>187</v>
       </c>
       <c r="E76" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F76" t="b">
         <v>1</v>
@@ -4493,19 +4493,16 @@
         <v>0</v>
       </c>
       <c r="K76" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="L76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N76" t="b">
         <v>0</v>
-      </c>
-      <c r="O76" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="77" spans="1:18">
@@ -4513,13 +4510,13 @@
         <v>28</v>
       </c>
       <c r="B77" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>128</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>128</v>
+        <v>188</v>
       </c>
       <c r="E77" t="b">
         <v>1</v>
@@ -4537,7 +4534,7 @@
         <v>0</v>
       </c>
       <c r="K77" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="L77" t="b">
         <v>0</v>
@@ -4547,6 +4544,9 @@
       </c>
       <c r="N77" t="b">
         <v>0</v>
+      </c>
+      <c r="O77" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="78" spans="1:18">
@@ -4557,10 +4557,10 @@
         <v>88</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D78" t="s">
-        <v>188</v>
+        <v>128</v>
       </c>
       <c r="E78" t="b">
         <v>1</v>
@@ -4578,7 +4578,7 @@
         <v>0</v>
       </c>
       <c r="K78" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="L78" t="b">
         <v>0</v>
@@ -4588,9 +4588,6 @@
       </c>
       <c r="N78" t="b">
         <v>0</v>
-      </c>
-      <c r="O78" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:18">
@@ -4601,7 +4598,7 @@
         <v>89</v>
       </c>
       <c r="C79" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="D79" t="s">
         <v>189</v>
@@ -4622,7 +4619,7 @@
         <v>0</v>
       </c>
       <c r="K79" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="L79" t="b">
         <v>0</v>
@@ -4645,7 +4642,7 @@
         <v>90</v>
       </c>
       <c r="C80" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="D80" t="s">
         <v>190</v>
@@ -4666,7 +4663,7 @@
         <v>0</v>
       </c>
       <c r="K80" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="L80" t="b">
         <v>0</v>
@@ -4676,6 +4673,9 @@
       </c>
       <c r="N80" t="b">
         <v>0</v>
+      </c>
+      <c r="O80" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="81" spans="1:15">
@@ -4686,7 +4686,7 @@
         <v>91</v>
       </c>
       <c r="C81" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="D81" t="s">
         <v>191</v>
@@ -4748,7 +4748,7 @@
         <v>0</v>
       </c>
       <c r="K82" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="L82" t="b">
         <v>0</v>
@@ -4758,9 +4758,6 @@
       </c>
       <c r="N82" t="b">
         <v>0</v>
-      </c>
-      <c r="O82" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="83" spans="1:15">
@@ -4771,7 +4768,7 @@
         <v>93</v>
       </c>
       <c r="C83" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="D83" t="s">
         <v>193</v>
@@ -4792,7 +4789,7 @@
         <v>0</v>
       </c>
       <c r="K83" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="L83" t="b">
         <v>0</v>
@@ -4802,6 +4799,9 @@
       </c>
       <c r="N83" t="b">
         <v>0</v>
+      </c>
+      <c r="O83" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="84" spans="1:15">
@@ -4812,7 +4812,7 @@
         <v>94</v>
       </c>
       <c r="C84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D84" t="s">
         <v>194</v>
@@ -4833,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="K84" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L84" t="b">
         <v>0</v>
@@ -4850,10 +4850,10 @@
         <v>28</v>
       </c>
       <c r="B85" t="s">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="C85" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D85" t="s">
         <v>195</v>
@@ -4874,7 +4874,7 @@
         <v>0</v>
       </c>
       <c r="K85" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="L85" t="b">
         <v>0</v>
@@ -4884,9 +4884,6 @@
       </c>
       <c r="N85" t="b">
         <v>0</v>
-      </c>
-      <c r="O85" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="86" spans="1:15">
@@ -4894,10 +4891,10 @@
         <v>28</v>
       </c>
       <c r="B86" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C86" t="s">
-        <v>108</v>
+        <v>133</v>
       </c>
       <c r="D86" t="s">
         <v>196</v>
@@ -4918,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="K86" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="L86" t="b">
         <v>0</v>
@@ -4930,7 +4927,7 @@
         <v>0</v>
       </c>
       <c r="O86" t="s">
-        <v>218</v>
+        <v>228</v>
       </c>
     </row>
     <row r="87" spans="1:15">
@@ -4938,13 +4935,13 @@
         <v>28</v>
       </c>
       <c r="B87" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C87" t="s">
         <v>109</v>
       </c>
       <c r="D87" t="s">
-        <v>109</v>
+        <v>197</v>
       </c>
       <c r="E87" t="b">
         <v>1</v>
@@ -4962,15 +4959,59 @@
         <v>0</v>
       </c>
       <c r="K87" t="s">
+        <v>207</v>
+      </c>
+      <c r="L87" t="b">
+        <v>0</v>
+      </c>
+      <c r="M87" t="b">
+        <v>0</v>
+      </c>
+      <c r="N87" t="b">
+        <v>0</v>
+      </c>
+      <c r="O87" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
+      <c r="A88" t="s">
+        <v>28</v>
+      </c>
+      <c r="B88" t="s">
+        <v>51</v>
+      </c>
+      <c r="C88" t="s">
+        <v>110</v>
+      </c>
+      <c r="D88" t="s">
+        <v>110</v>
+      </c>
+      <c r="E88" t="b">
+        <v>1</v>
+      </c>
+      <c r="F88" t="b">
+        <v>1</v>
+      </c>
+      <c r="G88" t="b">
+        <v>0</v>
+      </c>
+      <c r="I88" t="b">
+        <v>0</v>
+      </c>
+      <c r="J88" t="b">
+        <v>0</v>
+      </c>
+      <c r="K88" t="s">
         <v>199</v>
       </c>
-      <c r="L87" t="b">
-        <v>0</v>
-      </c>
-      <c r="M87" t="b">
-        <v>0</v>
-      </c>
-      <c r="N87" t="b">
+      <c r="L88" t="b">
+        <v>0</v>
+      </c>
+      <c r="M88" t="b">
+        <v>0</v>
+      </c>
+      <c r="N88" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>